<commit_message>
Added Get Value from Cart functionality and updated excel
</commit_message>
<xml_diff>
--- a/nopCommerce Automation Testing.xlsx
+++ b/nopCommerce Automation Testing.xlsx
@@ -1,18 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24923"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F540EA92-CCB2-4D01-B058-B10AE9286474}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="105" windowWidth="22995" windowHeight="9285" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="480" yWindow="105" windowWidth="20730" windowHeight="9285"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1 - Completed Tasks" sheetId="5" r:id="rId1"/>
-    <sheet name="Sheet3 - Workflow TCs" sheetId="3" r:id="rId2"/>
-    <sheet name="Sheet2 - Pending Tasks" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="124519"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -28,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="193">
   <si>
     <t>S. No</t>
   </si>
@@ -236,6 +233,22 @@
   </si>
   <si>
     <t>Registration fails and page shows appropriate message as "Password must meet the following rules:..."</t>
+  </si>
+  <si>
+    <t>Invalid Registration FirstName</t>
+  </si>
+  <si>
+    <t>1. Enter an invalid value in the firstname field.
+2. Click on Register button</t>
+  </si>
+  <si>
+    <t>Registration fails and page shows appropriate message "firstname should only contain letters"</t>
+  </si>
+  <si>
+    <t>Invalid Registration LastName</t>
+  </si>
+  <si>
+    <t>Registration fails and page shows appropriate message "lastname should only contain letters"</t>
   </si>
   <si>
     <t>Duplicate Registration</t>
@@ -498,23 +511,6 @@
 7. Green alert with successful addition to shopping cart is visible</t>
   </si>
   <si>
-    <t>1. Proceed To Clothing Page
-2. Proceed To Shoes Page
-3. View By Grid
-4. View By List
-5. Enter Add To Cart
-6. Select Item
-7. Select Size Option
-8. Verify No Size Error
-9.Verify Successful Addition
-10.Verify Positive Quantity Error
-11. Verify Enter Text Error Message
-12.Enter Quantity
-13.Add Clothes
-14.Add Custom Tshirt
-15.Add Nike Shirt</t>
-  </si>
-  <si>
     <t>1.none
 2.none
 3.none
@@ -644,6 +640,22 @@
 5. Negative or zero appears in textbox
 6.Item is added to cart 
 7. Negative quantity error appears in red color alert</t>
+  </si>
+  <si>
+    <t>Displaying Clothes In List View And Grid View</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Click on Apparel Link 
+2.Click on Clothing Link 
+3. Click on View by List Button 
+4. Click on View by Grid Button 
+</t>
+  </si>
+  <si>
+    <t>1. List of Items in Apparel :- Shoes,Clothing and Accessories is visible
+2. Products under clothing category are visible.
+3. Items are displayed as list.
+4. Items are displayed as grid.</t>
   </si>
   <si>
     <t>apparel_shoes</t>
@@ -912,24 +924,134 @@
 9. Red alert with negative quantity error is visible</t>
   </si>
   <si>
-    <t>S No.</t>
-  </si>
-  <si>
-    <t>Function Name</t>
-  </si>
-  <si>
-    <t>Input Arguments</t>
-  </si>
-  <si>
-    <t>nopCommerce
- demo store</t>
+    <t>Displaying Shoes In List View And Grid View</t>
+  </si>
+  <si>
+    <t>cart</t>
+  </si>
+  <si>
+    <t>Adding Adidas shoes and choosing gift wrap option</t>
+  </si>
+  <si>
+    <t>1.Add Adidas shoes to cart
+2. Check if shoes are added to cart
+3.Choose gift wrap option
+4.Check if gift wrap option is chosen
+5.Verify gift wrap option
+6.Agree to terms and conditions
+7.Checkout</t>
+  </si>
+  <si>
+    <t>1.Adidas shoes record is added to cart
+2.Gift wrap option is chosen
+3.Terms and conditions check box is chosen
+4.Page asking for sign in or register appears</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.Product name,size,color,print
+2.Product name, size ,color,custom text
+4.Product name
+16. New quantity
+</t>
+  </si>
+  <si>
+    <t>1-18. void</t>
+  </si>
+  <si>
+    <t>Adding Nike Floral Shoes and continue shopping</t>
+  </si>
+  <si>
+    <t>1.Nike Floral shoes are added to cart
+2.Check if shoes are added
+3.Continue shopping
+4.Check if Shoes page</t>
+  </si>
+  <si>
+    <t>1.Nike Floral shoes are added to cart
+2.Page showing shoes is shown after clicking on continue</t>
+  </si>
+  <si>
+    <t>Adding Nike Zoom Shoes and estimate shipping without giving country or zipcode</t>
+  </si>
+  <si>
+    <t>1.Nike Zoom shoes are added to cart
+2.Check if shoes are added
+3.Estimate shipping by filling details
+4.Chech is error message is displayed
+5.Check if shipping option changed</t>
+  </si>
+  <si>
+    <t>1.Nike Shoes are added to cart
+2.Shipping details are entered 
+3.Shipping price is updated</t>
+  </si>
+  <si>
+    <t>Removing custom shirt after adding to cart</t>
+  </si>
+  <si>
+    <t>1.Add Custom shirt
+2.Check if shirt is added
+3.Go to cart
+4.Remove item from cart
+5.Check if cart is empty</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.Custom shirt is added to cart.
+2.Page showing cart items appears.
+3Custom shirt is removed from cart.
+</t>
+  </si>
+  <si>
+    <t>Adding Nike shirt to cart and changing quantity to three</t>
+  </si>
+  <si>
+    <t>1.Add Nike shirt to cart
+2.Check if Nike shirt  is added to cart
+3.Change quantity to three
+4.Check if quantity has changed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.Nike shirt is added to cart
+2.Number of Nike shirts are updated
+</t>
+  </si>
+  <si>
+    <t>Adding Adidas shoes to cart and changing quantity to  minus three</t>
+  </si>
+  <si>
+    <t>1.Add Adidas shoes to cart
+2.Check if Adidas shoes  is added to cart
+3.Change quantity to  minus three
+4.Check if quantity error is shown</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.Adidas shoes are added to cart
+2.Number of Adidas shoes are not updated.Error is shown.
+</t>
+  </si>
+  <si>
+    <t>Adding Nike Zoom shoes to cart and changing quantity to zero</t>
+  </si>
+  <si>
+    <t>1.Add Nike Zoom shoes to cart
+2.Check if Nike Zoom shoes  is added to cart
+3.Change quantity to  zero
+4.Check if cart is empty</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.Nike Zoom shoes are added to cart
+2.Number of Nike Zoom shoes are not updated.It is removed from the cart.
+</t>
+  </si>
+  <si>
+    <t>workflow</t>
   </si>
   <si>
     <t>Shopping for Nike Shoes 
 As Guest Using Ground Shipping And Check Or Money Order Payment</t>
   </si>
   <si>
-    <t>1. Proceed to Apparel -&gt; Shoes page
+    <t xml:space="preserve">1. Proceed to Apparel -&gt; Shoes page
 2. Adding Nike Shoes to Cart by clicking on Add to Cart Button and selecting size,color and pattern.
 3. Checkout as Guest User
 4. Enter valid Billing Address fields and continue
@@ -938,10 +1060,10 @@
 7. Verify Payment Information
 8. Confirm the order
 9. View Order details
-10. Click on Download PDF Invoice</t>
-  </si>
-  <si>
-    <t>1. A page showing a grid of shoes appears
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. A page showing a grid of shoes appears
 2. Item is added into the Shopping Cart
 3. Checkout page appears
 4. Page shows shipping method options
@@ -950,7 +1072,7 @@
 7. Shows the billing and shipping address, and the products  bought along with options and price and tax information
 8. Checkout completed page opens up and the order number and a link to order details is visible
 9. Order Information is shown
-10. Order Information is downloaded as pdf file</t>
+</t>
   </si>
   <si>
     <t>Login:
@@ -1036,28 +1158,24 @@
 </t>
   </si>
   <si>
-    <t>nopCommerce
-demo store</t>
-  </si>
-  <si>
     <t xml:space="preserve">Shopping for Custom T-shirt As Registered User Using Next Day Air Shipping And Check Or Money Order Payment </t>
   </si>
   <si>
-    <t>0. Fill valid Registration form (also performs login)
-1. Verify Login Success
-2. Proceed to Apparel -&gt; Clothing page
-3. Add Custom t-Shirt to cart
-4. Checkout
-5. Enter valid Billing Address fields and continue
-6. Choose Next Day Air Shipping Method and continue
-7. Choose Check or Money Order Payment Method and continue
-8. Verify Payment Information
-9. Confirm the order
-10. View Order details
-111. Click on Download PDF Invoice</t>
-  </si>
-  <si>
-    <t>1. Login succeeds and page header shows an option to Log Out
+    <t xml:space="preserve">1. Fill valid Registration form (also performs login)
+2. Verify Login Success
+3. Proceed to Apparel -&gt; Clothing page
+4. Add Custom t-Shirt to cart
+5. Checkout
+6. Enter valid Billing Address fields and continue
+7. Choose Next Day Air Shipping Method and continue
+8. Choose Check or Money Order Payment Method and continue
+9. Verify Payment Information
+10. Confirm the order
+11. View Order details
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Login succeeds and page header shows an option to Log Out
 2. Webpage coressponding to all the clothing items
 3. Custom t-Shirt record is added into shopping cart
 4. Checkout page appears
@@ -1067,41 +1185,42 @@
 8. Shows the billing and shipping address, and the products  bought along with options and price and tax information
 9. Checkout completed page opens up and the order number and a link to order details is visible
 11. Order Information is shown
-12. Order information is downloaded as pdf file</t>
+</t>
   </si>
   <si>
     <t xml:space="preserve">Shopping for Nike T-shirt And Adidas Shoes As Registered User Using Next Day Air Shipping And Check Or Money Order Payment </t>
   </si>
   <si>
-    <t>0. Fill valid Registration form (also performs login)
-1. Verify Login Success
-2. Proceed to Apparel -&gt; Clothing page
-3. Add Nike T-Shirt to cart
-4. Go to Adidas Shoes page
-5. Add Adidas Shoes to cart
-6. Checkout
-7. Enter valid Billing Address fields and continue
-8. Choose Next Day Air Shipping Method and continue
-9. Choose Check or Money Order Payment Method and continue
-10. Verify Payment Information
-11. Confirm the order
-12. Click to view Order details
-13. Click on Download PDF Invoice</t>
-  </si>
-  <si>
-    <t>1. Login succeeds and home page opens with an option to Log Out
-2. Webpage showing a grid of clothes appears
-3. Nike t-Shirt record is added into shopping cart
-4. Webpage for adidas shoes shows up
-5. Adidas shoes record is added into shopping cart
-6. Checkout page appears
-7. Page shows shipping method options
-8.Payment Method list is shown
-9.Payment Information is printed
-10.Shows the billing and shipping address, and the products  bought along with options and price and tax information
-11.Checkout completed page opens up and the order number and a link to order details is visible
-12.Order Information is shown
-13.Order  information is downloaded as pdf file</t>
+    <t xml:space="preserve">1. Fill valid Registration form (also performs login)
+2. Verify Login Success
+3. Proceed to Apparel -&gt; Clothing page
+4. Add Nike T-Shirt to cart
+5. Go to Adidas Shoes page
+6. Add Adidas Shoes to cart
+7. Checkout
+8. Enter valid Billing Address fields and continue
+9. Choose Next Day Air Shipping Method and continue
+10. Choose Check or Money Order Payment Method and continue
+11. Verify Payment Information
+12. Confirm the order
+13. Click to view Order details
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Login succeeds and home page opens with an option to Log Out
+2. Successfully Logged in
+3. Webpage showing a grid of clothes appears
+4. Nike t-Shirt record is added into shopping cart
+5. Webpage for adidas shoes shows up
+6. Adidas shoes record is added into shopping cart
+7. Checkout page appears
+8. Page shows shipping method options
+9.Payment Method list is shown
+10.Payment Information is printed
+11.Shows the billing and shipping address, and the products  bought along with options and price and tax information
+12.Checkout completed page opens up and the order number and a link to order details is visible
+13.Order Information is shown
+</t>
   </si>
   <si>
     <t>Shopping for  shoes
@@ -1116,7 +1235,7 @@
 as a new user</t>
   </si>
   <si>
-    <t>1. Verify Valid Registraton
+    <t xml:space="preserve">1. Verify Valid Registraton
 2. Navigate to Apparel and then Shoes link
 3.Add Nike Floral Shoes with given attributes
 4. Go Back
@@ -1130,10 +1249,10 @@
 12.Verify Payment Information
 13.Verify Order Confirmation
 14.click to checkout details
-15.Download PDF Invoice</t>
-  </si>
-  <si>
-    <t>1. Registration succeeds and page shows "Your registration is complete" message, the user is logged in.Continue Button is visible.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Registration succeeds and page shows "Your registration is complete" message, the user is logged in.Continue Button is visible.
 2. Webpage coressponding to all the Apparel items
 3. Nike shoes page appears and all attributes are filled and added to cart
 4. Shoes page appears
@@ -1147,7 +1266,7 @@
 12.Payment Information is printed
 13.Checkout completed page opens up and the order number and a link to order details is visible
 14.Order Information is shown
-15.Order  information is downloaded as pdf file</t>
+</t>
   </si>
   <si>
     <t xml:space="preserve">Window Shopping for 
@@ -1179,10 +1298,10 @@
 10. logged out , homepage appears</t>
   </si>
   <si>
-    <t>Shopping for Shoes and Shirt as a registered user</t>
-  </si>
-  <si>
-    <t>1. Open Apparel webpage.
+    <t>Shopping for Shoes and Shirt as a new registered user(Registering After Shopping)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Open Apparel webpage.
 2. Move to shoes webpage.
 3. Select View by List 
 4. Add 2 NIke Zoom Shoes into Cart
@@ -1202,10 +1321,10 @@
 18.Verify Payment Information
 19.Verify Order Confirmation
 20.click to checkout details
-21.Download PDF Invoice</t>
-  </si>
-  <si>
-    <t>1. Apparel Webpage appears.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Apparel Webpage appears.
 2. Shoes webpage appears.
 3. Products are viewed as list
 4. 2 Nike Zoom Shoes are added into cart
@@ -1225,200 +1344,53 @@
 18. Order confirmation is visible
 19. Checkout completed page opens up and the order number and a link to order details is visible
 20.Order Information is shown
-21.Order  information is downloaded as pdf file</t>
-  </si>
-  <si>
-    <t>Input
- Arguments</t>
-  </si>
-  <si>
-    <t>cart</t>
-  </si>
-  <si>
-    <t>Removing custom shirt after adding and check out</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.Add Custom shirt
-2.Check if shirt is added
-3.Go to cart
-4.Remove item from cart
-5.Checkout </t>
-  </si>
-  <si>
-    <t>1.Custom shirt is added to cart.
-2.Page showing cart items appears.
-3Custom shirt is removed from cart.
-4.Page asking for sign in or register appears after check out</t>
-  </si>
-  <si>
-    <t>1.Select Item
- 2.Check Item In Cart
- 3. Enter Add To Cart
-4.Remove Item From Cart 
-5.Checkout</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.Product id of custom shirt
-2.Product name
-3.void
-4.Product Name
 </t>
   </si>
   <si>
-    <t xml:space="preserve">1.void
-2.Boolean
-3.void
-4.void
-5.void
-</t>
-  </si>
-  <si>
-    <t>Adding Adidas shoes and choosing gift wrap option</t>
-  </si>
-  <si>
-    <t>1.Add Adidas shoes to cart
-2. Check if shoes are added to cart
-3.Choose gift wrap option
-4.Check if gift wrap option is chosen
-5.Verify gift wrap option
-6.Agree to terms and conditions
-7.Checkout</t>
-  </si>
-  <si>
-    <t>1.Adidas shoes record is added to cart
-2.Gift wrap option is chosen
-3.Terms and conditions check box is chosen
-4.Page asking for sign in or register appears</t>
-  </si>
-  <si>
-    <t>1.Successfully Adding Adidas Shoes Into Cart
-2.Check Item In Cart
-3.Choose gift wrap
-4.Check Gift Wrap Chosen
-5.Click Terms And Conditions
-6.Verify Gift wrap option
-7.Checkout</t>
-  </si>
-  <si>
-    <t>1.void
-2.Product name
-3.gift wrap option
-4.void
-5.void
-6.void
-7.void</t>
-  </si>
-  <si>
-    <t>1.void
-2.Boolean
-3.void
-4.Boolean
-5.Boolean
-6.void</t>
-  </si>
-  <si>
-    <t>Adding Nike Floral Shoes and continue shopping</t>
-  </si>
-  <si>
-    <t>1.Nike Floral shoes are added to cart
-2.Check if shoes are added
-3.Continue shopping
-4.Check if Shoes page</t>
-  </si>
-  <si>
-    <t>1.Nike Floral shoes are added to cart
-2.Page showing shoes is shown after clicking on continue</t>
-  </si>
-  <si>
-    <t>1.Successfully Adding Nike Floral Shoes Into Cart
-2.Check Item In Cart
-3.Continue Shopping
-4.Check Which Page</t>
-  </si>
-  <si>
-    <t>1.void
-2.Product name
-3.void
-4.Page name</t>
-  </si>
-  <si>
-    <t>1.void
-2.Boolean
-3.void
-4.Boolean</t>
-  </si>
-  <si>
-    <t>Adding Nike Floral Shoes and estimate shipping without giving country or zipcode</t>
-  </si>
-  <si>
-    <t>1.Nike Floral shoes are added to cart
-2.Check if shoes are added
-3.Estimate shipping by filling details
-4.Chech is error message is displayed
-5.Check if shipping option changed</t>
-  </si>
-  <si>
-    <t>1.Nike Shoes are added to cart
-2.Shipping details are entered 
-3.Shipping price is updated</t>
-  </si>
-  <si>
-    <t>1.Successfully Adding Nike Floral Shoes Into Cart
-2.Check Item In Cart
-3.Estimate Shipping
-4.Check Error in shipping
-5.Check Shipping</t>
-  </si>
-  <si>
-    <t>1.void
-2.product name
-3.Country,Zipcode,shipping method
-4.Error List
-5.Shipping method</t>
-  </si>
-  <si>
-    <t>1.void
-2.Boolean
-3.void
-4.Boolean list
-5.Boolean</t>
-  </si>
-  <si>
-    <t>Adding Nike Zoom shoes to cart and changing quantity to three</t>
-  </si>
-  <si>
-    <t>1.Add Nike Zoom shoes to cart
-2.Check if Nike zoom shoes are added to cart
-3.Change quantity to three
-4.Check if quantity has changed</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.Nike Zoom shoes are added to cart
-2.Number of Nike shoes is updated
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.Successfully Adding Nike Zoom Shoes Into Cart
-2.Check Item In Cart
-3.Change Quantity in cart
-4.Check Quantity In Cart
-</t>
-  </si>
-  <si>
-    <t>1.void
-2.Product Name
-3.New_quantity
-4.Product name,quantity</t>
-  </si>
-  <si>
-    <t>Test case that fails</t>
+    <t>1. Proceed To Clothing Page
+2. Proceed To Shoes Page
+3. View By Grid
+4. View By List
+5. Enter Add To Cart
+6. Select Item
+7. Select Size Option
+8. Verify No Size Error
+9.Verify Successful Addition
+10.Verify Positive Quantity Error
+11. Verify Enter Text Error Message
+12.Enter Quantity
+13.Add Clothes
+14.Add Custom Tshirt
+15.Add Nike Shirt
+16. Find Price</t>
+  </si>
+  <si>
+    <t>1.Add Shoes
+2.Add Clothes
+3.Check Item In Cart
+4.Remove Item From Cart
+5.Check If Cart Is Empty
+6.Choose Giftwrap Option As Yes
+7.Verify Gift Wrap Option As Yes
+8.Select Term And Conditions
+9.Click Checkout Button 
+10.Click Estimate Shipping Button
+11.Click Apply Estimate Button
+12.Check Zipcode Error
+13.Check Country Error
+14.Click Continue Shopping Button
+15.Check If Shoes Page
+16.Change Quantity
+17.Check Quantity Error
+18.Proceed To Shopping Cart
+19. Get Total Cart Value</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1454,13 +1426,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -1491,7 +1456,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1528,6 +1493,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD0CECE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -1544,14 +1521,13 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -1582,38 +1558,44 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1633,82 +1615,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>762000</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>400050</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="3" name="TextBox 2">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{694126FE-807B-4A63-869D-FA481C141645}"/>
-            </a:ext>
-            <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
-              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{B0D23638-E699-4C67-8851-F494222EE09B}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="9039225" y="19269075"/>
-          <a:ext cx="2152650" cy="2971800"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="lt1"/>
-        </a:solidFill>
-        <a:ln w="9525" cmpd="sng">
-          <a:solidFill>
-            <a:schemeClr val="lt1">
-              <a:shade val="50000"/>
-            </a:schemeClr>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" lIns="91440" tIns="45720" rIns="91440" bIns="45720" rtlCol="0" anchor="t">
-          <a:noAutofit/>
-        </a:bodyPr>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr marL="0" indent="0" algn="l"/>
-          <a:endParaRPr lang="en-US" sz="1100">
-            <a:latin typeface="+mn-lt"/>
-            <a:ea typeface="+mn-lt"/>
-            <a:cs typeface="+mn-lt"/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:pPr marL="0" indent="0" algn="l"/>
-          <a:endParaRPr lang="en-US" sz="1100">
-            <a:latin typeface="+mn-lt"/>
-            <a:ea typeface="+mn-lt"/>
-            <a:cs typeface="+mn-lt"/>
-          </a:endParaRPr>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1754,7 +1660,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1786,27 +1692,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1838,24 +1726,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -2031,48 +1901,48 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01CB26F0-748C-463E-B635-3207BD00A4E2}">
-  <dimension ref="A1:H47"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:H66"/>
   <sheetViews>
-    <sheetView topLeftCell="A47" workbookViewId="0">
-      <selection activeCell="F40" sqref="F40:F47"/>
+    <sheetView tabSelected="1" topLeftCell="A53" workbookViewId="0">
+      <selection activeCell="E55" sqref="E55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="6" customWidth="1"/>
-    <col min="2" max="2" width="16.7109375" style="7" customWidth="1"/>
-    <col min="3" max="3" width="29" style="5" customWidth="1"/>
-    <col min="4" max="4" width="38.7109375" style="7" customWidth="1"/>
-    <col min="5" max="5" width="39.140625" style="5" customWidth="1"/>
-    <col min="6" max="6" width="46.42578125" style="7" customWidth="1"/>
-    <col min="7" max="7" width="25.7109375" style="7" customWidth="1"/>
-    <col min="8" max="8" width="30.7109375" style="7" customWidth="1"/>
+    <col min="2" max="2" width="16.7109375" style="6" customWidth="1"/>
+    <col min="3" max="3" width="29" style="4" customWidth="1"/>
+    <col min="4" max="4" width="38.7109375" style="6" customWidth="1"/>
+    <col min="5" max="5" width="39.140625" style="4" customWidth="1"/>
+    <col min="6" max="6" width="46.42578125" style="6" customWidth="1"/>
+    <col min="7" max="7" width="25.7109375" style="6" customWidth="1"/>
+    <col min="8" max="8" width="30.7109375" style="6" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="E1" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="G1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="H1" s="5" t="s">
         <v>7</v>
       </c>
     </row>
@@ -2080,25 +1950,25 @@
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="C2" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="21" t="s">
+      <c r="F2" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="G2" s="21" t="s">
+      <c r="G2" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="H2" s="21" t="s">
+      <c r="H2" s="22" t="s">
         <v>14</v>
       </c>
     </row>
@@ -2106,129 +1976,129 @@
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="11" t="s">
+      <c r="C3" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="E3" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="21"/>
-      <c r="G3" s="21"/>
-      <c r="H3" s="21"/>
+      <c r="F3" s="22"/>
+      <c r="G3" s="22"/>
+      <c r="H3" s="22"/>
     </row>
     <row r="4" spans="1:8" ht="35.25" customHeight="1">
       <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="11" t="s">
+      <c r="C4" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="E4" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="F4" s="21"/>
-      <c r="G4" s="21"/>
-      <c r="H4" s="21"/>
+      <c r="F4" s="22"/>
+      <c r="G4" s="22"/>
+      <c r="H4" s="22"/>
     </row>
     <row r="5" spans="1:8" ht="45">
       <c r="A5">
         <v>4</v>
       </c>
-      <c r="B5" s="9" t="s">
+      <c r="B5" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="11" t="s">
+      <c r="C5" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="D5" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="E5" s="5" t="s">
+      <c r="E5" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="F5" s="21"/>
-      <c r="G5" s="21"/>
-      <c r="H5" s="21"/>
+      <c r="F5" s="22"/>
+      <c r="G5" s="22"/>
+      <c r="H5" s="22"/>
     </row>
     <row r="6" spans="1:8" ht="45">
       <c r="A6">
         <v>5</v>
       </c>
-      <c r="B6" s="9" t="s">
+      <c r="B6" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="11" t="s">
+      <c r="C6" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="D6" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="E6" s="5" t="s">
+      <c r="E6" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="F6" s="21"/>
-      <c r="G6" s="21"/>
-      <c r="H6" s="21"/>
+      <c r="F6" s="22"/>
+      <c r="G6" s="22"/>
+      <c r="H6" s="22"/>
     </row>
     <row r="7" spans="1:8" ht="30">
       <c r="A7">
         <v>6</v>
       </c>
-      <c r="B7" s="9" t="s">
+      <c r="B7" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="11" t="s">
+      <c r="C7" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="D7" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="E7" s="5" t="s">
+      <c r="E7" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="F7" s="21"/>
-      <c r="G7" s="21"/>
-      <c r="H7" s="21"/>
+      <c r="F7" s="22"/>
+      <c r="G7" s="22"/>
+      <c r="H7" s="22"/>
     </row>
     <row r="8" spans="1:8" ht="23.25" customHeight="1">
-      <c r="F8" s="5"/>
-      <c r="G8" s="5"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="4"/>
     </row>
     <row r="9" spans="1:8" ht="29.25" customHeight="1">
       <c r="A9">
         <v>7</v>
       </c>
-      <c r="B9" s="12" t="s">
+      <c r="B9" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="C9" s="11" t="s">
+      <c r="C9" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="D9" s="5" t="s">
+      <c r="D9" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="E9" s="5" t="s">
+      <c r="E9" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="F9" s="21" t="s">
+      <c r="F9" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="G9" s="21" t="s">
+      <c r="G9" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="H9" s="21" t="s">
+      <c r="H9" s="22" t="s">
         <v>14</v>
       </c>
     </row>
@@ -2236,1123 +2106,1121 @@
       <c r="A10">
         <v>8</v>
       </c>
-      <c r="B10" s="12" t="s">
+      <c r="B10" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="C10" s="11" t="s">
+      <c r="C10" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="D10" s="5" t="s">
+      <c r="D10" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="E10" s="5" t="s">
+      <c r="E10" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="F10" s="21"/>
-      <c r="G10" s="21"/>
-      <c r="H10" s="21"/>
+      <c r="F10" s="22"/>
+      <c r="G10" s="22"/>
+      <c r="H10" s="22"/>
     </row>
     <row r="11" spans="1:8" ht="33" customHeight="1">
       <c r="A11">
         <v>9</v>
       </c>
-      <c r="B11" s="12" t="s">
+      <c r="B11" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="C11" s="11" t="s">
+      <c r="C11" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="D11" s="5" t="s">
+      <c r="D11" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="E11" s="5" t="s">
+      <c r="E11" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="F11" s="21"/>
-      <c r="G11" s="21"/>
-      <c r="H11" s="21"/>
+      <c r="F11" s="22"/>
+      <c r="G11" s="22"/>
+      <c r="H11" s="22"/>
     </row>
     <row r="12" spans="1:8" ht="33.75" customHeight="1">
       <c r="A12">
         <v>10</v>
       </c>
-      <c r="B12" s="12" t="s">
+      <c r="B12" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="C12" s="11" t="s">
+      <c r="C12" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="D12" s="5" t="s">
+      <c r="D12" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="E12" s="5" t="s">
+      <c r="E12" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="F12" s="21"/>
-      <c r="G12" s="21"/>
-      <c r="H12" s="21"/>
+      <c r="F12" s="22"/>
+      <c r="G12" s="22"/>
+      <c r="H12" s="22"/>
     </row>
     <row r="13" spans="1:8" ht="48.75" customHeight="1">
       <c r="A13">
         <v>11</v>
       </c>
-      <c r="B13" s="12" t="s">
+      <c r="B13" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="C13" s="11" t="s">
+      <c r="C13" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="D13" s="5" t="s">
+      <c r="D13" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="E13" s="5" t="s">
+      <c r="E13" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="F13" s="21"/>
-      <c r="G13" s="21"/>
-      <c r="H13" s="21"/>
-    </row>
-    <row r="14" spans="1:8" ht="80.25" customHeight="1">
+      <c r="F13" s="22"/>
+      <c r="G13" s="22"/>
+      <c r="H13" s="22"/>
+    </row>
+    <row r="14" spans="1:8" ht="48.75" customHeight="1">
       <c r="A14">
         <v>12</v>
       </c>
-      <c r="B14" s="12" t="s">
+      <c r="B14" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="C14" s="11" t="s">
+      <c r="C14" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="D14" s="5" t="s">
+      <c r="D14" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="E14" s="5" t="s">
+      <c r="E14" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="F14" s="21"/>
-      <c r="G14" s="21"/>
-      <c r="H14" s="21"/>
-    </row>
-    <row r="15" spans="1:8" ht="29.25" customHeight="1">
-      <c r="C15" s="11"/>
-      <c r="D15" s="5"/>
-      <c r="F15" s="5"/>
-      <c r="G15" s="5"/>
-      <c r="H15" s="5"/>
-    </row>
-    <row r="16" spans="1:8" ht="37.5" customHeight="1">
+      <c r="F14" s="22"/>
+      <c r="G14" s="22"/>
+      <c r="H14" s="22"/>
+    </row>
+    <row r="15" spans="1:8" ht="48.75" customHeight="1">
+      <c r="A15">
+        <v>13</v>
+      </c>
+      <c r="B15" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="C15" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="F15" s="22"/>
+      <c r="G15" s="22"/>
+      <c r="H15" s="22"/>
+    </row>
+    <row r="16" spans="1:8" ht="80.25" customHeight="1">
       <c r="A16">
-        <v>13</v>
-      </c>
-      <c r="B16" s="13" t="s">
-        <v>50</v>
-      </c>
-      <c r="C16" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="D16" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="C16" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="E16" s="5" t="s">
+      <c r="D16" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="F16" s="21" t="s">
+      <c r="E16" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="G16" s="21" t="s">
-        <v>55</v>
-      </c>
-      <c r="H16" s="21" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" ht="78.75" customHeight="1">
-      <c r="A17">
-        <v>14</v>
-      </c>
-      <c r="B17" s="13" t="s">
-        <v>50</v>
-      </c>
-      <c r="C17" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="D17" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="E17" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="F17" s="21"/>
-      <c r="G17" s="21"/>
-      <c r="H17" s="21"/>
-    </row>
-    <row r="18" spans="1:8" ht="95.25" customHeight="1">
+      <c r="F16" s="22"/>
+      <c r="G16" s="22"/>
+      <c r="H16" s="22"/>
+    </row>
+    <row r="17" spans="1:8" ht="29.25" customHeight="1">
+      <c r="C17" s="10"/>
+      <c r="D17" s="4"/>
+      <c r="F17" s="4"/>
+      <c r="G17" s="4"/>
+      <c r="H17" s="4"/>
+    </row>
+    <row r="18" spans="1:8" ht="37.5" customHeight="1">
       <c r="A18">
         <v>15</v>
       </c>
-      <c r="B18" s="13" t="s">
-        <v>50</v>
-      </c>
-      <c r="C18" s="5" t="s">
+      <c r="B18" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="F18" s="22" t="s">
         <v>59</v>
       </c>
-      <c r="D18" s="5" t="s">
+      <c r="G18" s="22" t="s">
         <v>60</v>
       </c>
-      <c r="E18" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="F18" s="21"/>
-      <c r="G18" s="21"/>
-      <c r="H18" s="21"/>
-    </row>
-    <row r="19" spans="1:8" ht="42.75" customHeight="1">
+      <c r="H18" s="22" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="78.75" customHeight="1">
       <c r="A19">
         <v>16</v>
       </c>
-      <c r="B19" s="13" t="s">
-        <v>50</v>
-      </c>
-      <c r="C19" s="5" t="s">
+      <c r="B19" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="D19" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="D19" s="5" t="s">
+      <c r="E19" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="E19" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="F19" s="21"/>
-      <c r="G19" s="21"/>
-      <c r="H19" s="21"/>
-    </row>
-    <row r="20" spans="1:8" ht="57.75" customHeight="1">
+      <c r="F19" s="22"/>
+      <c r="G19" s="22"/>
+      <c r="H19" s="22"/>
+    </row>
+    <row r="20" spans="1:8" ht="95.25" customHeight="1">
       <c r="A20">
         <v>17</v>
       </c>
-      <c r="B20" s="13" t="s">
-        <v>50</v>
-      </c>
-      <c r="C20" s="5" t="s">
+      <c r="B20" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="D20" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="D20" s="5" t="s">
+      <c r="E20" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="E20" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="F20" s="21"/>
-      <c r="G20" s="21"/>
-      <c r="H20" s="21"/>
-    </row>
-    <row r="21" spans="1:8" ht="56.25" customHeight="1">
+      <c r="F20" s="22"/>
+      <c r="G20" s="22"/>
+      <c r="H20" s="22"/>
+    </row>
+    <row r="21" spans="1:8" ht="42.75" customHeight="1">
       <c r="A21">
         <v>18</v>
       </c>
-      <c r="B21" s="13" t="s">
-        <v>50</v>
-      </c>
-      <c r="C21" s="5" t="s">
+      <c r="B21" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="D21" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="D21" s="5" t="s">
+      <c r="E21" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="E21" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="F21" s="21"/>
-      <c r="G21" s="21"/>
-      <c r="H21" s="21"/>
-    </row>
-    <row r="22" spans="1:8" ht="35.25" customHeight="1">
+      <c r="F21" s="22"/>
+      <c r="G21" s="22"/>
+      <c r="H21" s="22"/>
+    </row>
+    <row r="22" spans="1:8" ht="57.75" customHeight="1">
       <c r="A22">
         <v>19</v>
       </c>
-      <c r="B22" s="13" t="s">
-        <v>50</v>
-      </c>
-      <c r="C22" s="5" t="s">
+      <c r="B22" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="D22" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="D22" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="E22" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="F22" s="21"/>
-      <c r="G22" s="21"/>
-      <c r="H22" s="21"/>
-    </row>
-    <row r="23" spans="1:8" ht="51" customHeight="1">
+      <c r="E22" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="F22" s="22"/>
+      <c r="G22" s="22"/>
+      <c r="H22" s="22"/>
+    </row>
+    <row r="23" spans="1:8" ht="56.25" customHeight="1">
       <c r="A23">
         <v>20</v>
       </c>
-      <c r="B23" s="13" t="s">
-        <v>50</v>
-      </c>
-      <c r="C23" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="D23" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="E23" s="5" t="s">
+      <c r="B23" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="C23" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="F23" s="21"/>
-      <c r="G23" s="21"/>
-      <c r="H23" s="21"/>
-    </row>
-    <row r="24" spans="1:8" ht="38.25" customHeight="1">
+      <c r="D23" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="F23" s="22"/>
+      <c r="G23" s="22"/>
+      <c r="H23" s="22"/>
+    </row>
+    <row r="24" spans="1:8" ht="35.25" customHeight="1">
       <c r="A24">
         <v>21</v>
       </c>
-      <c r="B24" s="13" t="s">
-        <v>50</v>
-      </c>
-      <c r="C24" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="D24" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="E24" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="F24" s="21"/>
-      <c r="G24" s="21"/>
-      <c r="H24" s="21"/>
-    </row>
-    <row r="25" spans="1:8" ht="54.75" customHeight="1">
+      <c r="B24" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="E24" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="F24" s="22"/>
+      <c r="G24" s="22"/>
+      <c r="H24" s="22"/>
+    </row>
+    <row r="25" spans="1:8" ht="51" customHeight="1">
       <c r="A25">
         <v>22</v>
       </c>
-      <c r="B25" s="13" t="s">
-        <v>50</v>
-      </c>
-      <c r="C25" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="D25" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="E25" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="F25" s="21"/>
-      <c r="G25" s="21"/>
-      <c r="H25" s="21"/>
-    </row>
-    <row r="26" spans="1:8" ht="104.25" customHeight="1">
+      <c r="B25" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="E25" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="F25" s="22"/>
+      <c r="G25" s="22"/>
+      <c r="H25" s="22"/>
+    </row>
+    <row r="26" spans="1:8" ht="38.25" customHeight="1">
       <c r="A26">
         <v>23</v>
       </c>
-      <c r="B26" s="13" t="s">
-        <v>50</v>
-      </c>
-      <c r="C26" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="D26" s="5" t="s">
+      <c r="B26" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="E26" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="E26" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="F26" s="21"/>
-      <c r="G26" s="21"/>
-      <c r="H26" s="21"/>
-    </row>
-    <row r="27" spans="1:8" ht="105">
+      <c r="F26" s="22"/>
+      <c r="G26" s="22"/>
+      <c r="H26" s="22"/>
+    </row>
+    <row r="27" spans="1:8" ht="54.75" customHeight="1">
       <c r="A27">
         <v>24</v>
       </c>
-      <c r="B27" s="13" t="s">
-        <v>50</v>
-      </c>
-      <c r="C27" s="5" t="s">
+      <c r="B27" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="C27" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="D27" s="5" t="s">
+      <c r="D27" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="E27" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="E27" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="F27" s="21"/>
-      <c r="G27" s="21"/>
-      <c r="H27" s="21"/>
-    </row>
-    <row r="28" spans="1:8" ht="120">
+      <c r="F27" s="22"/>
+      <c r="G27" s="22"/>
+      <c r="H27" s="22"/>
+    </row>
+    <row r="28" spans="1:8" ht="104.25" customHeight="1">
       <c r="A28">
         <v>25</v>
       </c>
-      <c r="B28" s="13" t="s">
-        <v>50</v>
-      </c>
-      <c r="C28" s="5" t="s">
+      <c r="B28" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="D28" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="D28" s="5" t="s">
+      <c r="E28" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="E28" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="F28" s="21"/>
-      <c r="G28" s="21"/>
-      <c r="H28" s="21"/>
-    </row>
-    <row r="29" spans="1:8" ht="103.5" customHeight="1">
+      <c r="F28" s="22"/>
+      <c r="G28" s="22"/>
+      <c r="H28" s="22"/>
+    </row>
+    <row r="29" spans="1:8" ht="105">
       <c r="A29">
         <v>26</v>
       </c>
-      <c r="B29" s="13" t="s">
-        <v>50</v>
-      </c>
-      <c r="C29" s="5" t="s">
+      <c r="B29" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="C29" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="D29" s="5" t="s">
+      <c r="D29" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="E29" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="F29" s="21"/>
-      <c r="G29" s="21"/>
-      <c r="H29" s="21"/>
+      <c r="E29" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="F29" s="22"/>
+      <c r="G29" s="22"/>
+      <c r="H29" s="22"/>
     </row>
     <row r="30" spans="1:8" ht="120">
       <c r="A30">
         <v>27</v>
       </c>
-      <c r="B30" s="13" t="s">
-        <v>50</v>
-      </c>
-      <c r="C30" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="D30" s="5" t="s">
+      <c r="B30" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="D30" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="E30" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="E30" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="F30" s="21"/>
-      <c r="G30" s="21"/>
-      <c r="H30" s="21"/>
-    </row>
-    <row r="31" spans="1:8" ht="120">
+      <c r="F30" s="22"/>
+      <c r="G30" s="22"/>
+      <c r="H30" s="22"/>
+    </row>
+    <row r="31" spans="1:8" ht="103.5" customHeight="1">
       <c r="A31">
         <v>28</v>
       </c>
-      <c r="B31" s="13" t="s">
-        <v>50</v>
-      </c>
-      <c r="C31" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="D31" s="5" t="s">
+      <c r="B31" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="D31" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="E31" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="F31" s="22"/>
+      <c r="G31" s="22"/>
+      <c r="H31" s="22"/>
+    </row>
+    <row r="32" spans="1:8" ht="120">
+      <c r="A32">
+        <v>29</v>
+      </c>
+      <c r="B32" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="D32" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="E31" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="F31" s="21"/>
-      <c r="G31" s="21"/>
-      <c r="H31" s="21"/>
-    </row>
-    <row r="32" spans="1:8" ht="33.75" customHeight="1">
-      <c r="F32" s="5"/>
-      <c r="G32" s="5"/>
-      <c r="H32" s="5"/>
-    </row>
-    <row r="33" spans="1:8" ht="148.5" customHeight="1">
+      <c r="E32" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="F32" s="22"/>
+      <c r="G32" s="22"/>
+      <c r="H32" s="22"/>
+    </row>
+    <row r="33" spans="1:8" ht="120">
       <c r="A33">
-        <v>29</v>
-      </c>
-      <c r="B33" s="14" t="s">
-        <v>90</v>
-      </c>
-      <c r="C33" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="D33" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="E33" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B33" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="C33" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="F33" s="21" t="s">
+      <c r="D33" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="G33" s="21" t="s">
-        <v>95</v>
-      </c>
-      <c r="H33" s="23" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" ht="150">
-      <c r="A34">
-        <v>30</v>
-      </c>
-      <c r="B34" s="14" t="s">
-        <v>90</v>
-      </c>
-      <c r="C34" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="D34" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="E34" s="5" t="s">
-        <v>98</v>
-      </c>
-      <c r="F34" s="21"/>
-      <c r="G34" s="21"/>
-      <c r="H34" s="23"/>
-    </row>
-    <row r="35" spans="1:8" ht="216" customHeight="1">
+      <c r="E33" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="F33" s="22"/>
+      <c r="G33" s="22"/>
+      <c r="H33" s="22"/>
+    </row>
+    <row r="34" spans="1:8" ht="33.75" customHeight="1">
+      <c r="F34" s="4"/>
+      <c r="G34" s="4"/>
+      <c r="H34" s="4"/>
+    </row>
+    <row r="35" spans="1:8" ht="148.5" customHeight="1">
       <c r="A35">
         <v>31</v>
       </c>
-      <c r="B35" s="14" t="s">
-        <v>90</v>
-      </c>
-      <c r="C35" s="5" t="s">
+      <c r="B35" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="C35" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="D35" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="E35" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="F35" s="22" t="s">
+        <v>191</v>
+      </c>
+      <c r="G35" s="22" t="s">
         <v>99</v>
       </c>
-      <c r="D35" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="E35" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="F35" s="21"/>
-      <c r="G35" s="21"/>
-      <c r="H35" s="23"/>
+      <c r="H35" s="26" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="36" spans="1:8" ht="150">
       <c r="A36">
         <v>32</v>
       </c>
-      <c r="B36" s="14" t="s">
-        <v>90</v>
-      </c>
-      <c r="C36" s="5" t="s">
+      <c r="B36" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="C36" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="D36" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="E36" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="D36" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="E36" s="5" t="s">
-        <v>104</v>
-      </c>
-      <c r="F36" s="21"/>
-      <c r="G36" s="21"/>
-      <c r="H36" s="23"/>
-    </row>
-    <row r="37" spans="1:8" ht="157.5" customHeight="1">
+      <c r="F36" s="22"/>
+      <c r="G36" s="22"/>
+      <c r="H36" s="26"/>
+    </row>
+    <row r="37" spans="1:8" ht="216" customHeight="1">
       <c r="A37">
         <v>33</v>
       </c>
-      <c r="B37" s="14" t="s">
-        <v>90</v>
-      </c>
-      <c r="C37" s="5" t="s">
+      <c r="B37" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="C37" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="D37" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="E37" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="D37" s="15" t="s">
-        <v>106</v>
-      </c>
-      <c r="E37" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="F37" s="21"/>
-      <c r="G37" s="21"/>
-      <c r="H37" s="23"/>
+      <c r="F37" s="22"/>
+      <c r="G37" s="22"/>
+      <c r="H37" s="26"/>
     </row>
     <row r="38" spans="1:8" ht="150">
       <c r="A38">
         <v>34</v>
       </c>
-      <c r="B38" s="14" t="s">
-        <v>90</v>
-      </c>
-      <c r="C38" s="5" t="s">
+      <c r="B38" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="C38" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="D38" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="E38" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="D38" s="15" t="s">
+      <c r="F38" s="22"/>
+      <c r="G38" s="22"/>
+      <c r="H38" s="26"/>
+    </row>
+    <row r="39" spans="1:8" ht="157.5" customHeight="1">
+      <c r="A39">
+        <v>35</v>
+      </c>
+      <c r="B39" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="C39" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="E38" s="5" t="s">
+      <c r="D39" s="14" t="s">
         <v>110</v>
       </c>
-      <c r="F38" s="21"/>
-      <c r="G38" s="21"/>
-      <c r="H38" s="23"/>
-    </row>
-    <row r="39" spans="1:8" ht="29.25" customHeight="1"/>
-    <row r="40" spans="1:8" ht="255" customHeight="1">
+      <c r="E39" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="F39" s="22"/>
+      <c r="G39" s="22"/>
+      <c r="H39" s="26"/>
+    </row>
+    <row r="40" spans="1:8" ht="150">
       <c r="A40">
-        <v>35</v>
-      </c>
-      <c r="B40" s="20" t="s">
-        <v>111</v>
-      </c>
-      <c r="C40" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B40" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="C40" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="D40" s="15" t="s">
+      <c r="D40" s="14" t="s">
         <v>113</v>
       </c>
-      <c r="E40" s="5" t="s">
+      <c r="E40" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="F40" s="21" t="s">
+      <c r="F40" s="22"/>
+      <c r="G40" s="22"/>
+      <c r="H40" s="26"/>
+    </row>
+    <row r="41" spans="1:8" ht="90">
+      <c r="A41">
+        <v>37</v>
+      </c>
+      <c r="B41" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="C41" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="G40" s="21" t="s">
+      <c r="D41" s="14" t="s">
         <v>116</v>
       </c>
-      <c r="H40" s="22" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" ht="195">
-      <c r="A41">
-        <v>36</v>
-      </c>
-      <c r="B41" s="20" t="s">
-        <v>111</v>
-      </c>
-      <c r="C41" s="5" t="s">
+      <c r="E41" s="4" t="s">
         <v>117</v>
       </c>
-      <c r="D41" s="15" t="s">
-        <v>118</v>
-      </c>
-      <c r="E41" s="5" t="s">
-        <v>119</v>
-      </c>
-      <c r="F41" s="21"/>
-      <c r="G41" s="21"/>
-      <c r="H41" s="22"/>
-    </row>
-    <row r="42" spans="1:8" ht="150">
-      <c r="A42">
-        <v>37</v>
-      </c>
-      <c r="B42" s="20" t="s">
-        <v>111</v>
-      </c>
-      <c r="C42" s="5" t="s">
-        <v>120</v>
-      </c>
-      <c r="D42" s="15" t="s">
-        <v>121</v>
-      </c>
-      <c r="E42" s="5" t="s">
-        <v>122</v>
-      </c>
-      <c r="F42" s="21"/>
-      <c r="G42" s="21"/>
-      <c r="H42" s="22"/>
-    </row>
-    <row r="43" spans="1:8" ht="409.6">
+      <c r="F41" s="22"/>
+      <c r="G41" s="4"/>
+      <c r="H41" s="17"/>
+    </row>
+    <row r="42" spans="1:8" ht="29.25" customHeight="1"/>
+    <row r="43" spans="1:8" ht="255" customHeight="1">
       <c r="A43">
         <v>38</v>
       </c>
-      <c r="B43" s="20" t="s">
-        <v>111</v>
-      </c>
-      <c r="C43" s="5" t="s">
+      <c r="B43" s="16" t="s">
+        <v>118</v>
+      </c>
+      <c r="C43" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="D43" s="14" t="s">
+        <v>120</v>
+      </c>
+      <c r="E43" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="F43" s="22" t="s">
+        <v>122</v>
+      </c>
+      <c r="G43" s="22" t="s">
         <v>123</v>
       </c>
-      <c r="D43" s="15" t="s">
-        <v>124</v>
-      </c>
-      <c r="E43" s="5" t="s">
-        <v>125</v>
-      </c>
-      <c r="F43" s="21"/>
-      <c r="G43" s="21"/>
-      <c r="H43" s="22"/>
-    </row>
-    <row r="44" spans="1:8" ht="165">
+      <c r="H43" s="25" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" ht="195">
       <c r="A44">
         <v>39</v>
       </c>
-      <c r="B44" s="20" t="s">
-        <v>111</v>
-      </c>
-      <c r="C44" s="5" t="s">
+      <c r="B44" s="16" t="s">
+        <v>118</v>
+      </c>
+      <c r="C44" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="D44" s="14" t="s">
+        <v>125</v>
+      </c>
+      <c r="E44" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="D44" s="15" t="s">
-        <v>127</v>
-      </c>
-      <c r="E44" s="5" t="s">
-        <v>128</v>
-      </c>
-      <c r="F44" s="21"/>
-      <c r="G44" s="21"/>
-      <c r="H44" s="22"/>
-    </row>
-    <row r="45" spans="1:8" ht="180">
+      <c r="F44" s="22"/>
+      <c r="G44" s="22"/>
+      <c r="H44" s="25"/>
+    </row>
+    <row r="45" spans="1:8" ht="150">
       <c r="A45">
         <v>40</v>
       </c>
-      <c r="B45" s="20" t="s">
-        <v>111</v>
-      </c>
-      <c r="C45" s="5" t="s">
+      <c r="B45" s="16" t="s">
+        <v>118</v>
+      </c>
+      <c r="C45" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="D45" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="E45" s="4" t="s">
         <v>129</v>
       </c>
-      <c r="D45" s="15" t="s">
-        <v>130</v>
-      </c>
-      <c r="E45" s="5" t="s">
-        <v>131</v>
-      </c>
-      <c r="F45" s="21"/>
-      <c r="G45" s="21"/>
-      <c r="H45" s="22"/>
-    </row>
-    <row r="46" spans="1:8" ht="180">
+      <c r="F45" s="22"/>
+      <c r="G45" s="22"/>
+      <c r="H45" s="25"/>
+    </row>
+    <row r="46" spans="1:8" ht="409.6" customHeight="1">
       <c r="A46">
         <v>41</v>
       </c>
-      <c r="B46" s="20" t="s">
-        <v>111</v>
-      </c>
-      <c r="C46" s="5" t="s">
+      <c r="B46" s="16" t="s">
+        <v>118</v>
+      </c>
+      <c r="C46" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="D46" s="14" t="s">
+        <v>131</v>
+      </c>
+      <c r="E46" s="4" t="s">
         <v>132</v>
       </c>
-      <c r="D46" s="15" t="s">
-        <v>133</v>
-      </c>
-      <c r="E46" s="5" t="s">
-        <v>134</v>
-      </c>
-      <c r="F46" s="21"/>
-      <c r="G46" s="21"/>
-      <c r="H46" s="22"/>
-    </row>
-    <row r="47" spans="1:8" ht="195">
+      <c r="F46" s="22"/>
+      <c r="G46" s="22"/>
+      <c r="H46" s="25"/>
+    </row>
+    <row r="47" spans="1:8" ht="165">
       <c r="A47">
         <v>42</v>
       </c>
-      <c r="B47" s="20" t="s">
-        <v>111</v>
-      </c>
-      <c r="C47" s="5" t="s">
+      <c r="B47" s="16" t="s">
+        <v>118</v>
+      </c>
+      <c r="C47" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="D47" s="14" t="s">
+        <v>134</v>
+      </c>
+      <c r="E47" s="4" t="s">
         <v>135</v>
       </c>
-      <c r="D47" s="15" t="s">
+      <c r="F47" s="22"/>
+      <c r="G47" s="22"/>
+      <c r="H47" s="25"/>
+    </row>
+    <row r="48" spans="1:8" ht="180">
+      <c r="A48">
+        <v>43</v>
+      </c>
+      <c r="B48" s="16" t="s">
+        <v>118</v>
+      </c>
+      <c r="C48" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="E47" s="5" t="s">
+      <c r="D48" s="14" t="s">
         <v>137</v>
       </c>
-      <c r="F47" s="21"/>
-      <c r="G47" s="21"/>
-      <c r="H47" s="22"/>
+      <c r="E48" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="F48" s="22"/>
+      <c r="G48" s="22"/>
+      <c r="H48" s="25"/>
+    </row>
+    <row r="49" spans="1:8" ht="180">
+      <c r="A49">
+        <v>44</v>
+      </c>
+      <c r="B49" s="16" t="s">
+        <v>118</v>
+      </c>
+      <c r="C49" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="D49" s="14" t="s">
+        <v>140</v>
+      </c>
+      <c r="E49" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="F49" s="22"/>
+      <c r="G49" s="22"/>
+      <c r="H49" s="25"/>
+    </row>
+    <row r="50" spans="1:8" ht="195">
+      <c r="A50">
+        <v>45</v>
+      </c>
+      <c r="B50" s="16" t="s">
+        <v>118</v>
+      </c>
+      <c r="C50" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="D50" s="14" t="s">
+        <v>143</v>
+      </c>
+      <c r="E50" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="F50" s="22"/>
+      <c r="G50" s="22"/>
+      <c r="H50" s="25"/>
+    </row>
+    <row r="51" spans="1:8" ht="90">
+      <c r="A51">
+        <v>46</v>
+      </c>
+      <c r="B51" s="16" t="s">
+        <v>118</v>
+      </c>
+      <c r="C51" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="D51" s="14" t="s">
+        <v>116</v>
+      </c>
+      <c r="E51" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="F51" s="22"/>
+      <c r="G51" s="4"/>
+    </row>
+    <row r="52" spans="1:8">
+      <c r="B52" s="18"/>
+      <c r="D52" s="14"/>
+      <c r="F52" s="4"/>
+      <c r="G52" s="4"/>
+    </row>
+    <row r="53" spans="1:8" ht="120.75" customHeight="1">
+      <c r="A53" s="2">
+        <v>47</v>
+      </c>
+      <c r="B53" s="19" t="s">
+        <v>146</v>
+      </c>
+      <c r="C53" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="D53" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="E53" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="F53" s="22" t="s">
+        <v>192</v>
+      </c>
+      <c r="G53" s="22" t="s">
+        <v>150</v>
+      </c>
+      <c r="H53" s="22" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" ht="75" customHeight="1">
+      <c r="A54">
+        <v>48</v>
+      </c>
+      <c r="B54" s="19" t="s">
+        <v>146</v>
+      </c>
+      <c r="C54" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="D54" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="E54" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="F54" s="22"/>
+      <c r="G54" s="22"/>
+      <c r="H54" s="22"/>
+    </row>
+    <row r="55" spans="1:8" ht="120" customHeight="1">
+      <c r="A55">
+        <v>49</v>
+      </c>
+      <c r="B55" s="19" t="s">
+        <v>146</v>
+      </c>
+      <c r="C55" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="D55" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="E55" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="F55" s="22"/>
+      <c r="G55" s="22"/>
+      <c r="H55" s="22"/>
+    </row>
+    <row r="56" spans="1:8" ht="98.25" customHeight="1">
+      <c r="A56" s="2">
+        <v>50</v>
+      </c>
+      <c r="B56" s="19" t="s">
+        <v>146</v>
+      </c>
+      <c r="C56" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="D56" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="E56" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="F56" s="22"/>
+      <c r="G56" s="22"/>
+      <c r="H56" s="22"/>
+    </row>
+    <row r="57" spans="1:8" ht="75" customHeight="1">
+      <c r="A57">
+        <v>51</v>
+      </c>
+      <c r="B57" s="19" t="s">
+        <v>146</v>
+      </c>
+      <c r="C57" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="D57" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="E57" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="F57" s="22"/>
+      <c r="G57" s="22"/>
+      <c r="H57" s="22"/>
+    </row>
+    <row r="58" spans="1:8" ht="90" customHeight="1">
+      <c r="A58">
+        <v>52</v>
+      </c>
+      <c r="B58" s="19" t="s">
+        <v>146</v>
+      </c>
+      <c r="C58" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="D58" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="E58" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="F58" s="22"/>
+      <c r="G58" s="22"/>
+      <c r="H58" s="22"/>
+    </row>
+    <row r="59" spans="1:8" ht="75">
+      <c r="A59">
+        <v>53</v>
+      </c>
+      <c r="B59" s="19" t="s">
+        <v>146</v>
+      </c>
+      <c r="C59" s="4" t="s">
+        <v>167</v>
+      </c>
+      <c r="D59" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="E59" s="4" t="s">
+        <v>169</v>
+      </c>
+      <c r="F59" s="22"/>
+      <c r="G59" s="22"/>
+      <c r="H59" s="22"/>
+    </row>
+    <row r="60" spans="1:8">
+      <c r="B60" s="20"/>
+      <c r="D60" s="4"/>
+      <c r="F60" s="4"/>
+      <c r="G60" s="4"/>
+      <c r="H60" s="4"/>
+    </row>
+    <row r="61" spans="1:8" ht="225">
+      <c r="A61" s="3">
+        <v>54</v>
+      </c>
+      <c r="B61" s="21" t="s">
+        <v>170</v>
+      </c>
+      <c r="C61" s="15" t="s">
+        <v>171</v>
+      </c>
+      <c r="D61" s="15" t="s">
+        <v>172</v>
+      </c>
+      <c r="E61" s="15" t="s">
+        <v>173</v>
+      </c>
+      <c r="F61" s="23" t="s">
+        <v>174</v>
+      </c>
+      <c r="G61" s="23" t="s">
+        <v>175</v>
+      </c>
+      <c r="H61" s="23" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" ht="270">
+      <c r="A62" s="3">
+        <v>55</v>
+      </c>
+      <c r="B62" s="21" t="s">
+        <v>170</v>
+      </c>
+      <c r="C62" s="15" t="s">
+        <v>176</v>
+      </c>
+      <c r="D62" s="15" t="s">
+        <v>177</v>
+      </c>
+      <c r="E62" s="15" t="s">
+        <v>178</v>
+      </c>
+      <c r="F62" s="24"/>
+      <c r="G62" s="23"/>
+      <c r="H62" s="23"/>
+    </row>
+    <row r="63" spans="1:8" ht="345">
+      <c r="A63" s="3">
+        <v>56</v>
+      </c>
+      <c r="B63" s="21" t="s">
+        <v>170</v>
+      </c>
+      <c r="C63" s="15" t="s">
+        <v>179</v>
+      </c>
+      <c r="D63" s="15" t="s">
+        <v>180</v>
+      </c>
+      <c r="E63" s="15" t="s">
+        <v>181</v>
+      </c>
+      <c r="F63" s="24"/>
+      <c r="G63" s="23"/>
+      <c r="H63" s="23"/>
+    </row>
+    <row r="64" spans="1:8" ht="375">
+      <c r="A64" s="3">
+        <v>57</v>
+      </c>
+      <c r="B64" s="21" t="s">
+        <v>170</v>
+      </c>
+      <c r="C64" s="15" t="s">
+        <v>182</v>
+      </c>
+      <c r="D64" s="15" t="s">
+        <v>183</v>
+      </c>
+      <c r="E64" s="15" t="s">
+        <v>184</v>
+      </c>
+      <c r="F64" s="24"/>
+      <c r="G64" s="23"/>
+      <c r="H64" s="23"/>
+    </row>
+    <row r="65" spans="1:8" ht="255">
+      <c r="A65">
+        <v>58</v>
+      </c>
+      <c r="B65" s="21" t="s">
+        <v>170</v>
+      </c>
+      <c r="C65" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="D65" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="E65" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="F65" s="24"/>
+      <c r="G65" s="23"/>
+      <c r="H65" s="23"/>
+    </row>
+    <row r="66" spans="1:8" ht="390">
+      <c r="A66">
+        <v>59</v>
+      </c>
+      <c r="B66" s="21" t="s">
+        <v>170</v>
+      </c>
+      <c r="C66" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="D66" s="14" t="s">
+        <v>189</v>
+      </c>
+      <c r="E66" s="4" t="s">
+        <v>190</v>
+      </c>
+      <c r="F66" s="24"/>
+      <c r="G66" s="23"/>
+      <c r="H66" s="23"/>
     </row>
   </sheetData>
-  <mergeCells count="15">
-    <mergeCell ref="F40:F47"/>
-    <mergeCell ref="G40:G47"/>
-    <mergeCell ref="H40:H47"/>
-    <mergeCell ref="F33:F38"/>
+  <mergeCells count="21">
+    <mergeCell ref="F61:F66"/>
+    <mergeCell ref="G61:G66"/>
+    <mergeCell ref="H61:H66"/>
+    <mergeCell ref="F35:F41"/>
+    <mergeCell ref="G43:G50"/>
+    <mergeCell ref="H43:H50"/>
+    <mergeCell ref="G35:G40"/>
+    <mergeCell ref="H35:H40"/>
+    <mergeCell ref="F43:F51"/>
+    <mergeCell ref="F53:F59"/>
+    <mergeCell ref="G53:G59"/>
+    <mergeCell ref="H53:H59"/>
     <mergeCell ref="F2:F7"/>
     <mergeCell ref="G2:G7"/>
     <mergeCell ref="H2:H7"/>
-    <mergeCell ref="G16:G31"/>
-    <mergeCell ref="H16:H31"/>
-    <mergeCell ref="F9:F14"/>
-    <mergeCell ref="G9:G14"/>
-    <mergeCell ref="H9:H14"/>
-    <mergeCell ref="F16:F31"/>
-    <mergeCell ref="G33:G38"/>
-    <mergeCell ref="H33:H38"/>
+    <mergeCell ref="G18:G33"/>
+    <mergeCell ref="H18:H33"/>
+    <mergeCell ref="F9:F16"/>
+    <mergeCell ref="G9:G16"/>
+    <mergeCell ref="H9:H16"/>
+    <mergeCell ref="F18:F33"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:H7"/>
-  <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="5.42578125" customWidth="1"/>
-    <col min="2" max="2" width="11.85546875" style="7" customWidth="1"/>
-    <col min="3" max="3" width="19.5703125" style="5" customWidth="1"/>
-    <col min="4" max="4" width="44.5703125" style="7" customWidth="1"/>
-    <col min="5" max="5" width="50.85546875" style="7" customWidth="1"/>
-    <col min="6" max="6" width="51.140625" style="7" customWidth="1"/>
-    <col min="7" max="7" width="48.42578125" style="7" customWidth="1"/>
-    <col min="8" max="8" width="29" style="7" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8" ht="18.75" customHeight="1">
-      <c r="A1" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="B1" s="16" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="16" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="16" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="16" t="s">
-        <v>139</v>
-      </c>
-      <c r="G1" s="17" t="s">
-        <v>140</v>
-      </c>
-      <c r="H1" s="16" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" ht="196.5" customHeight="1">
-      <c r="A2" s="4">
-        <v>1</v>
-      </c>
-      <c r="B2" s="18" t="s">
-        <v>141</v>
-      </c>
-      <c r="C2" s="19" t="s">
-        <v>142</v>
-      </c>
-      <c r="D2" s="19" t="s">
-        <v>143</v>
-      </c>
-      <c r="E2" s="19" t="s">
-        <v>144</v>
-      </c>
-      <c r="F2" s="24" t="s">
-        <v>145</v>
-      </c>
-      <c r="G2" s="24" t="s">
-        <v>146</v>
-      </c>
-      <c r="H2" s="24" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" ht="269.25" customHeight="1">
-      <c r="A3" s="4">
-        <v>2</v>
-      </c>
-      <c r="B3" s="18" t="s">
-        <v>147</v>
-      </c>
-      <c r="C3" s="19" t="s">
-        <v>148</v>
-      </c>
-      <c r="D3" s="19" t="s">
-        <v>149</v>
-      </c>
-      <c r="E3" s="19" t="s">
-        <v>150</v>
-      </c>
-      <c r="F3" s="25"/>
-      <c r="G3" s="24"/>
-      <c r="H3" s="24"/>
-    </row>
-    <row r="4" spans="1:8" ht="269.25" customHeight="1">
-      <c r="A4" s="4">
-        <v>3</v>
-      </c>
-      <c r="B4" s="18" t="s">
-        <v>147</v>
-      </c>
-      <c r="C4" s="19" t="s">
-        <v>151</v>
-      </c>
-      <c r="D4" s="19" t="s">
-        <v>152</v>
-      </c>
-      <c r="E4" s="19" t="s">
-        <v>153</v>
-      </c>
-      <c r="F4" s="25"/>
-      <c r="G4" s="24"/>
-      <c r="H4" s="24"/>
-    </row>
-    <row r="5" spans="1:8" ht="354.75" customHeight="1">
-      <c r="A5" s="4">
-        <v>4</v>
-      </c>
-      <c r="B5" s="18" t="s">
-        <v>147</v>
-      </c>
-      <c r="C5" s="19" t="s">
-        <v>154</v>
-      </c>
-      <c r="D5" s="19" t="s">
-        <v>155</v>
-      </c>
-      <c r="E5" s="19" t="s">
-        <v>156</v>
-      </c>
-      <c r="F5" s="25"/>
-      <c r="G5" s="24"/>
-      <c r="H5" s="24"/>
-    </row>
-    <row r="6" spans="1:8" ht="214.5" customHeight="1">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6" s="18" t="s">
-        <v>147</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>157</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>158</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>159</v>
-      </c>
-      <c r="F6" s="25"/>
-      <c r="G6" s="24"/>
-      <c r="H6" s="24"/>
-    </row>
-    <row r="7" spans="1:8" ht="328.5" customHeight="1">
-      <c r="A7">
-        <v>6</v>
-      </c>
-      <c r="B7" s="18" t="s">
-        <v>147</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>160</v>
-      </c>
-      <c r="D7" s="15" t="s">
-        <v>161</v>
-      </c>
-      <c r="E7" s="5" t="s">
-        <v>162</v>
-      </c>
-      <c r="F7" s="25"/>
-      <c r="G7" s="24"/>
-      <c r="H7" s="24"/>
-    </row>
-  </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="F2:F7"/>
-    <mergeCell ref="G2:G7"/>
-    <mergeCell ref="H2:H7"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:H7"/>
-  <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="5.7109375" customWidth="1"/>
-    <col min="2" max="2" width="7.140625" style="7" customWidth="1"/>
-    <col min="3" max="3" width="18.140625" style="5" customWidth="1"/>
-    <col min="4" max="4" width="32.85546875" style="7" customWidth="1"/>
-    <col min="5" max="5" width="42.42578125" style="7" customWidth="1"/>
-    <col min="6" max="6" width="40.140625" style="7" customWidth="1"/>
-    <col min="7" max="7" width="21.85546875" style="7" customWidth="1"/>
-    <col min="8" max="8" width="12.28515625" style="7" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8" ht="30">
-      <c r="A1" s="16" t="s">
-        <v>138</v>
-      </c>
-      <c r="B1" s="16" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="16" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="16" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="16" t="s">
-        <v>139</v>
-      </c>
-      <c r="G1" s="17" t="s">
-        <v>163</v>
-      </c>
-      <c r="H1" s="16" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" ht="98.25" customHeight="1">
-      <c r="A2" s="2">
-        <v>1</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>164</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>165</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>166</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>167</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>168</v>
-      </c>
-      <c r="G2" s="5" t="s">
-        <v>169</v>
-      </c>
-      <c r="H2" s="5" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" ht="120.75" customHeight="1">
-      <c r="A3" s="2">
-        <v>2</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>164</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>171</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>172</v>
-      </c>
-      <c r="E3" s="5" t="s">
-        <v>173</v>
-      </c>
-      <c r="F3" s="5" t="s">
-        <v>174</v>
-      </c>
-      <c r="G3" s="5" t="s">
-        <v>175</v>
-      </c>
-      <c r="H3" s="5" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="75">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>164</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>177</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>178</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>179</v>
-      </c>
-      <c r="F4" s="5" t="s">
-        <v>180</v>
-      </c>
-      <c r="G4" s="5" t="s">
-        <v>181</v>
-      </c>
-      <c r="H4" s="5" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="120">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>164</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>183</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>184</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>185</v>
-      </c>
-      <c r="F5" s="5" t="s">
-        <v>186</v>
-      </c>
-      <c r="G5" s="5" t="s">
-        <v>187</v>
-      </c>
-      <c r="H5" s="5" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="90">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>164</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>189</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>190</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>191</v>
-      </c>
-      <c r="F6" s="5" t="s">
-        <v>192</v>
-      </c>
-      <c r="G6" s="5" t="s">
-        <v>193</v>
-      </c>
-      <c r="H6" s="5" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8">
-      <c r="A7">
-        <v>6</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>194</v>
-      </c>
-    </row>
-  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -3367,12 +3235,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A1DF0959A465604798737C0CF613A5FF" ma:contentTypeVersion="5" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="32a0f909cf80920549211a222706aa33">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="06292192-c18b-431d-898a-445811617056" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ccf405facfa43f58e2849d5976289537" ns2:_="">
     <xsd:import namespace="06292192-c18b-431d-898a-445811617056"/>
@@ -3522,14 +3384,43 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B3D6D229-377B-4744-BD35-CC0F5042A698}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B3D6D229-377B-4744-BD35-CC0F5042A698}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{78AF8109-82A3-433D-A366-A9063953868A}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F7944A00-B904-4D0F-8057-E221948F0A64}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="06292192-c18b-431d-898a-445811617056"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F7944A00-B904-4D0F-8057-E221948F0A64}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{78AF8109-82A3-433D-A366-A9063953868A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>